<commit_message>
floripa corrigido baseline (#129)
floripa corrigido baseline
</commit_message>
<xml_diff>
--- a/data/Florianopolis.xlsx
+++ b/data/Florianopolis.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Dropbox\Modelacao Brasil\CEA\CEA\Florianopolis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7526820-0840-493F-A72A-7C467DE65526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metrics" sheetId="1" r:id="rId1"/>
@@ -13,12 +19,12 @@
     <sheet name="scenarios_metadata" sheetId="4" r:id="rId4"/>
     <sheet name="log" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="483">
   <si>
     <t>Building_Name</t>
   </si>
@@ -1472,8 +1478,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1549,13 +1555,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1593,7 +1607,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1627,6 +1641,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1661,9 +1676,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1836,14 +1852,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE328"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1938,7 +1954,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -2033,7 +2049,7 @@
         <v>6663</v>
       </c>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2128,7 +2144,7 @@
         <v>2213</v>
       </c>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -2223,7 +2239,7 @@
         <v>26016</v>
       </c>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -2318,7 +2334,7 @@
         <v>29467</v>
       </c>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -2413,7 +2429,7 @@
         <v>9620</v>
       </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -2508,7 +2524,7 @@
         <v>4752</v>
       </c>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -2603,7 +2619,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -2638,7 +2654,7 @@
         <v>1356</v>
       </c>
       <c r="L9">
-        <v>8172.000000000001</v>
+        <v>8172.0000000000009</v>
       </c>
       <c r="M9">
         <v>3770</v>
@@ -2692,13 +2708,13 @@
         <v>1356</v>
       </c>
       <c r="AD9">
-        <v>8159.000000000001</v>
+        <v>8159.0000000000009</v>
       </c>
       <c r="AE9">
         <v>3776</v>
       </c>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -2793,7 +2809,7 @@
         <v>5904</v>
       </c>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -2888,7 +2904,7 @@
         <v>2411</v>
       </c>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -2983,7 +2999,7 @@
         <v>8623</v>
       </c>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -3078,7 +3094,7 @@
         <v>2669</v>
       </c>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -3173,7 +3189,7 @@
         <v>5871</v>
       </c>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -3268,7 +3284,7 @@
         <v>3713</v>
       </c>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -3363,7 +3379,7 @@
         <v>2126</v>
       </c>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -3458,7 +3474,7 @@
         <v>4468</v>
       </c>
     </row>
-    <row r="18" spans="1:31">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -3553,7 +3569,7 @@
         <v>1452</v>
       </c>
     </row>
-    <row r="19" spans="1:31">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -3648,7 +3664,7 @@
         <v>3137</v>
       </c>
     </row>
-    <row r="20" spans="1:31">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -3743,7 +3759,7 @@
         <v>2547</v>
       </c>
     </row>
-    <row r="21" spans="1:31">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -3778,7 +3794,7 @@
         <v>4220</v>
       </c>
       <c r="L21">
-        <v>8063.000000000001</v>
+        <v>8063.0000000000009</v>
       </c>
       <c r="M21">
         <v>2470</v>
@@ -3838,7 +3854,7 @@
         <v>2569</v>
       </c>
     </row>
-    <row r="22" spans="1:31">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -3933,7 +3949,7 @@
         <v>2443</v>
       </c>
     </row>
-    <row r="23" spans="1:31">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -4028,7 +4044,7 @@
         <v>4283</v>
       </c>
     </row>
-    <row r="24" spans="1:31">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -4123,7 +4139,7 @@
         <v>3857</v>
       </c>
     </row>
-    <row r="25" spans="1:31">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -4218,7 +4234,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="26" spans="1:31">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -4313,7 +4329,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="27" spans="1:31">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -4408,7 +4424,7 @@
         <v>2136</v>
       </c>
     </row>
-    <row r="28" spans="1:31">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -4503,7 +4519,7 @@
         <v>2837</v>
       </c>
     </row>
-    <row r="29" spans="1:31">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -4598,7 +4614,7 @@
         <v>1909</v>
       </c>
     </row>
-    <row r="30" spans="1:31">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -4693,7 +4709,7 @@
         <v>17733</v>
       </c>
     </row>
-    <row r="31" spans="1:31">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -4788,7 +4804,7 @@
         <v>2917</v>
       </c>
     </row>
-    <row r="32" spans="1:31">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -4883,7 +4899,7 @@
         <v>4306</v>
       </c>
     </row>
-    <row r="33" spans="1:31">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -4978,7 +4994,7 @@
         <v>25553</v>
       </c>
     </row>
-    <row r="34" spans="1:31">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -5073,7 +5089,7 @@
         <v>3085</v>
       </c>
     </row>
-    <row r="35" spans="1:31">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -5168,7 +5184,7 @@
         <v>6983</v>
       </c>
     </row>
-    <row r="36" spans="1:31">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -5263,7 +5279,7 @@
         <v>1764</v>
       </c>
     </row>
-    <row r="37" spans="1:31">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>66</v>
       </c>
@@ -5358,7 +5374,7 @@
         <v>2078</v>
       </c>
     </row>
-    <row r="38" spans="1:31">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>67</v>
       </c>
@@ -5453,7 +5469,7 @@
         <v>3064</v>
       </c>
     </row>
-    <row r="39" spans="1:31">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>68</v>
       </c>
@@ -5548,7 +5564,7 @@
         <v>4852</v>
       </c>
     </row>
-    <row r="40" spans="1:31">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>69</v>
       </c>
@@ -5643,7 +5659,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="41" spans="1:31">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -5738,7 +5754,7 @@
         <v>2756</v>
       </c>
     </row>
-    <row r="42" spans="1:31">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>71</v>
       </c>
@@ -5833,7 +5849,7 @@
         <v>11670</v>
       </c>
     </row>
-    <row r="43" spans="1:31">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -5928,7 +5944,7 @@
         <v>1856</v>
       </c>
     </row>
-    <row r="44" spans="1:31">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>73</v>
       </c>
@@ -5981,7 +5997,7 @@
         <v>4493</v>
       </c>
       <c r="R44">
-        <v>8183.999999999999</v>
+        <v>8183.9999999999991</v>
       </c>
       <c r="S44">
         <v>982</v>
@@ -6023,7 +6039,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="45" spans="1:31">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>74</v>
       </c>
@@ -6118,7 +6134,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="46" spans="1:31">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>75</v>
       </c>
@@ -6213,7 +6229,7 @@
         <v>5120</v>
       </c>
     </row>
-    <row r="47" spans="1:31">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>76</v>
       </c>
@@ -6308,7 +6324,7 @@
         <v>3341</v>
       </c>
     </row>
-    <row r="48" spans="1:31">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>77</v>
       </c>
@@ -6403,7 +6419,7 @@
         <v>1951</v>
       </c>
     </row>
-    <row r="49" spans="1:31">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>78</v>
       </c>
@@ -6498,7 +6514,7 @@
         <v>10307</v>
       </c>
     </row>
-    <row r="50" spans="1:31">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>79</v>
       </c>
@@ -6593,7 +6609,7 @@
         <v>6659</v>
       </c>
     </row>
-    <row r="51" spans="1:31">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>80</v>
       </c>
@@ -6688,7 +6704,7 @@
         <v>1868</v>
       </c>
     </row>
-    <row r="52" spans="1:31">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>81</v>
       </c>
@@ -6783,7 +6799,7 @@
         <v>9738</v>
       </c>
     </row>
-    <row r="53" spans="1:31">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>82</v>
       </c>
@@ -6878,7 +6894,7 @@
         <v>2041</v>
       </c>
     </row>
-    <row r="54" spans="1:31">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>83</v>
       </c>
@@ -6973,7 +6989,7 @@
         <v>14825</v>
       </c>
     </row>
-    <row r="55" spans="1:31">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>84</v>
       </c>
@@ -7068,7 +7084,7 @@
         <v>2705</v>
       </c>
     </row>
-    <row r="56" spans="1:31">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>85</v>
       </c>
@@ -7163,7 +7179,7 @@
         <v>3201</v>
       </c>
     </row>
-    <row r="57" spans="1:31">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>86</v>
       </c>
@@ -7258,7 +7274,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="58" spans="1:31">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>87</v>
       </c>
@@ -7353,7 +7369,7 @@
         <v>4378</v>
       </c>
     </row>
-    <row r="59" spans="1:31">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>88</v>
       </c>
@@ -7448,7 +7464,7 @@
         <v>10747</v>
       </c>
     </row>
-    <row r="60" spans="1:31">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>89</v>
       </c>
@@ -7543,7 +7559,7 @@
         <v>4831</v>
       </c>
     </row>
-    <row r="61" spans="1:31">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>90</v>
       </c>
@@ -7638,7 +7654,7 @@
         <v>3790</v>
       </c>
     </row>
-    <row r="62" spans="1:31">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>91</v>
       </c>
@@ -7733,7 +7749,7 @@
         <v>3314</v>
       </c>
     </row>
-    <row r="63" spans="1:31">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>92</v>
       </c>
@@ -7828,7 +7844,7 @@
         <v>2682</v>
       </c>
     </row>
-    <row r="64" spans="1:31">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>93</v>
       </c>
@@ -7923,7 +7939,7 @@
         <v>2295</v>
       </c>
     </row>
-    <row r="65" spans="1:31">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>94</v>
       </c>
@@ -8018,7 +8034,7 @@
         <v>2808</v>
       </c>
     </row>
-    <row r="66" spans="1:31">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>95</v>
       </c>
@@ -8113,7 +8129,7 @@
         <v>2493</v>
       </c>
     </row>
-    <row r="67" spans="1:31">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>96</v>
       </c>
@@ -8208,7 +8224,7 @@
         <v>7060</v>
       </c>
     </row>
-    <row r="68" spans="1:31">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>97</v>
       </c>
@@ -8303,7 +8319,7 @@
         <v>1907</v>
       </c>
     </row>
-    <row r="69" spans="1:31">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>98</v>
       </c>
@@ -8398,7 +8414,7 @@
         <v>8220</v>
       </c>
     </row>
-    <row r="70" spans="1:31">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>99</v>
       </c>
@@ -8493,7 +8509,7 @@
         <v>4298</v>
       </c>
     </row>
-    <row r="71" spans="1:31">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>100</v>
       </c>
@@ -8588,7 +8604,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="72" spans="1:31">
+    <row r="72" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>101</v>
       </c>
@@ -8683,7 +8699,7 @@
         <v>3512</v>
       </c>
     </row>
-    <row r="73" spans="1:31">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>102</v>
       </c>
@@ -8742,7 +8758,7 @@
         <v>1375</v>
       </c>
       <c r="T73">
-        <v>8087.999999999999</v>
+        <v>8087.9999999999991</v>
       </c>
       <c r="U73">
         <v>5501</v>
@@ -8778,7 +8794,7 @@
         <v>3348</v>
       </c>
     </row>
-    <row r="74" spans="1:31">
+    <row r="74" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>103</v>
       </c>
@@ -8873,7 +8889,7 @@
         <v>3658</v>
       </c>
     </row>
-    <row r="75" spans="1:31">
+    <row r="75" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>104</v>
       </c>
@@ -8926,7 +8942,7 @@
         <v>4421</v>
       </c>
       <c r="R75">
-        <v>8013.999999999999</v>
+        <v>8013.9999999999991</v>
       </c>
       <c r="S75">
         <v>988</v>
@@ -8968,7 +8984,7 @@
         <v>2278</v>
       </c>
     </row>
-    <row r="76" spans="1:31">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>105</v>
       </c>
@@ -9063,7 +9079,7 @@
         <v>3420</v>
       </c>
     </row>
-    <row r="77" spans="1:31">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>106</v>
       </c>
@@ -9158,7 +9174,7 @@
         <v>3645</v>
       </c>
     </row>
-    <row r="78" spans="1:31">
+    <row r="78" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>107</v>
       </c>
@@ -9253,7 +9269,7 @@
         <v>4314</v>
       </c>
     </row>
-    <row r="79" spans="1:31">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>108</v>
       </c>
@@ -9348,7 +9364,7 @@
         <v>2392</v>
       </c>
     </row>
-    <row r="80" spans="1:31">
+    <row r="80" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>109</v>
       </c>
@@ -9443,7 +9459,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="81" spans="1:31">
+    <row r="81" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>110</v>
       </c>
@@ -9538,7 +9554,7 @@
         <v>2214</v>
       </c>
     </row>
-    <row r="82" spans="1:31">
+    <row r="82" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>111</v>
       </c>
@@ -9633,7 +9649,7 @@
         <v>2404</v>
       </c>
     </row>
-    <row r="83" spans="1:31">
+    <row r="83" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>112</v>
       </c>
@@ -9728,7 +9744,7 @@
         <v>2118</v>
       </c>
     </row>
-    <row r="84" spans="1:31">
+    <row r="84" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>113</v>
       </c>
@@ -9823,7 +9839,7 @@
         <v>1803</v>
       </c>
     </row>
-    <row r="85" spans="1:31">
+    <row r="85" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>114</v>
       </c>
@@ -9918,7 +9934,7 @@
         <v>2712</v>
       </c>
     </row>
-    <row r="86" spans="1:31">
+    <row r="86" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>115</v>
       </c>
@@ -10013,7 +10029,7 @@
         <v>4474</v>
       </c>
     </row>
-    <row r="87" spans="1:31">
+    <row r="87" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>116</v>
       </c>
@@ -10108,7 +10124,7 @@
         <v>4101</v>
       </c>
     </row>
-    <row r="88" spans="1:31">
+    <row r="88" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>117</v>
       </c>
@@ -10203,7 +10219,7 @@
         <v>3112</v>
       </c>
     </row>
-    <row r="89" spans="1:31">
+    <row r="89" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>118</v>
       </c>
@@ -10298,7 +10314,7 @@
         <v>5635</v>
       </c>
     </row>
-    <row r="90" spans="1:31">
+    <row r="90" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>119</v>
       </c>
@@ -10393,7 +10409,7 @@
         <v>6892</v>
       </c>
     </row>
-    <row r="91" spans="1:31">
+    <row r="91" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>120</v>
       </c>
@@ -10488,7 +10504,7 @@
         <v>7603</v>
       </c>
     </row>
-    <row r="92" spans="1:31">
+    <row r="92" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>121</v>
       </c>
@@ -10583,7 +10599,7 @@
         <v>2128</v>
       </c>
     </row>
-    <row r="93" spans="1:31">
+    <row r="93" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>122</v>
       </c>
@@ -10678,7 +10694,7 @@
         <v>8909</v>
       </c>
     </row>
-    <row r="94" spans="1:31">
+    <row r="94" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>123</v>
       </c>
@@ -10773,7 +10789,7 @@
         <v>1804</v>
       </c>
     </row>
-    <row r="95" spans="1:31">
+    <row r="95" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>124</v>
       </c>
@@ -10868,7 +10884,7 @@
         <v>3234</v>
       </c>
     </row>
-    <row r="96" spans="1:31">
+    <row r="96" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>125</v>
       </c>
@@ -10963,7 +10979,7 @@
         <v>4070</v>
       </c>
     </row>
-    <row r="97" spans="1:31">
+    <row r="97" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>126</v>
       </c>
@@ -11058,7 +11074,7 @@
         <v>4328</v>
       </c>
     </row>
-    <row r="98" spans="1:31">
+    <row r="98" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>127</v>
       </c>
@@ -11153,7 +11169,7 @@
         <v>3076</v>
       </c>
     </row>
-    <row r="99" spans="1:31">
+    <row r="99" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>128</v>
       </c>
@@ -11248,7 +11264,7 @@
         <v>5296</v>
       </c>
     </row>
-    <row r="100" spans="1:31">
+    <row r="100" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>129</v>
       </c>
@@ -11343,7 +11359,7 @@
         <v>9842</v>
       </c>
     </row>
-    <row r="101" spans="1:31">
+    <row r="101" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>130</v>
       </c>
@@ -11438,7 +11454,7 @@
         <v>4952</v>
       </c>
     </row>
-    <row r="102" spans="1:31">
+    <row r="102" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>131</v>
       </c>
@@ -11533,7 +11549,7 @@
         <v>1597</v>
       </c>
     </row>
-    <row r="103" spans="1:31">
+    <row r="103" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>132</v>
       </c>
@@ -11628,7 +11644,7 @@
         <v>5291</v>
       </c>
     </row>
-    <row r="104" spans="1:31">
+    <row r="104" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>133</v>
       </c>
@@ -11723,7 +11739,7 @@
         <v>9846</v>
       </c>
     </row>
-    <row r="105" spans="1:31">
+    <row r="105" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>134</v>
       </c>
@@ -11818,7 +11834,7 @@
         <v>7317</v>
       </c>
     </row>
-    <row r="106" spans="1:31">
+    <row r="106" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>135</v>
       </c>
@@ -11913,7 +11929,7 @@
         <v>5699</v>
       </c>
     </row>
-    <row r="107" spans="1:31">
+    <row r="107" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>136</v>
       </c>
@@ -12008,7 +12024,7 @@
         <v>8196</v>
       </c>
     </row>
-    <row r="108" spans="1:31">
+    <row r="108" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>137</v>
       </c>
@@ -12103,7 +12119,7 @@
         <v>4801</v>
       </c>
     </row>
-    <row r="109" spans="1:31">
+    <row r="109" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>138</v>
       </c>
@@ -12198,7 +12214,7 @@
         <v>4188</v>
       </c>
     </row>
-    <row r="110" spans="1:31">
+    <row r="110" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>139</v>
       </c>
@@ -12293,7 +12309,7 @@
         <v>8307</v>
       </c>
     </row>
-    <row r="111" spans="1:31">
+    <row r="111" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>140</v>
       </c>
@@ -12388,7 +12404,7 @@
         <v>2199</v>
       </c>
     </row>
-    <row r="112" spans="1:31">
+    <row r="112" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>141</v>
       </c>
@@ -12483,7 +12499,7 @@
         <v>2810</v>
       </c>
     </row>
-    <row r="113" spans="1:31">
+    <row r="113" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>142</v>
       </c>
@@ -12578,7 +12594,7 @@
         <v>3256</v>
       </c>
     </row>
-    <row r="114" spans="1:31">
+    <row r="114" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>143</v>
       </c>
@@ -12673,7 +12689,7 @@
         <v>11746</v>
       </c>
     </row>
-    <row r="115" spans="1:31">
+    <row r="115" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>144</v>
       </c>
@@ -12708,7 +12724,7 @@
         <v>5679</v>
       </c>
       <c r="L115">
-        <v>8164.999999999999</v>
+        <v>8164.9999999999991</v>
       </c>
       <c r="M115">
         <v>2448</v>
@@ -12768,7 +12784,7 @@
         <v>2529</v>
       </c>
     </row>
-    <row r="116" spans="1:31">
+    <row r="116" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>145</v>
       </c>
@@ -12863,7 +12879,7 @@
         <v>2129</v>
       </c>
     </row>
-    <row r="117" spans="1:31">
+    <row r="117" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>146</v>
       </c>
@@ -12958,7 +12974,7 @@
         <v>2899</v>
       </c>
     </row>
-    <row r="118" spans="1:31">
+    <row r="118" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>147</v>
       </c>
@@ -13053,7 +13069,7 @@
         <v>2772</v>
       </c>
     </row>
-    <row r="119" spans="1:31">
+    <row r="119" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>148</v>
       </c>
@@ -13148,7 +13164,7 @@
         <v>6785</v>
       </c>
     </row>
-    <row r="120" spans="1:31">
+    <row r="120" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>149</v>
       </c>
@@ -13243,7 +13259,7 @@
         <v>11080</v>
       </c>
     </row>
-    <row r="121" spans="1:31">
+    <row r="121" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>150</v>
       </c>
@@ -13338,7 +13354,7 @@
         <v>14308</v>
       </c>
     </row>
-    <row r="122" spans="1:31">
+    <row r="122" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>151</v>
       </c>
@@ -13379,7 +13395,7 @@
         <v>2044</v>
       </c>
       <c r="N122">
-        <v>8031.000000000001</v>
+        <v>8031.0000000000009</v>
       </c>
       <c r="O122">
         <v>6053</v>
@@ -13433,7 +13449,7 @@
         <v>2038</v>
       </c>
     </row>
-    <row r="123" spans="1:31">
+    <row r="123" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>152</v>
       </c>
@@ -13528,7 +13544,7 @@
         <v>2615</v>
       </c>
     </row>
-    <row r="124" spans="1:31">
+    <row r="124" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>153</v>
       </c>
@@ -13623,7 +13639,7 @@
         <v>1782</v>
       </c>
     </row>
-    <row r="125" spans="1:31">
+    <row r="125" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>154</v>
       </c>
@@ -13718,7 +13734,7 @@
         <v>1871</v>
       </c>
     </row>
-    <row r="126" spans="1:31">
+    <row r="126" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>155</v>
       </c>
@@ -13813,7 +13829,7 @@
         <v>1625</v>
       </c>
     </row>
-    <row r="127" spans="1:31">
+    <row r="127" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>156</v>
       </c>
@@ -13908,7 +13924,7 @@
         <v>4178</v>
       </c>
     </row>
-    <row r="128" spans="1:31">
+    <row r="128" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>157</v>
       </c>
@@ -14003,7 +14019,7 @@
         <v>3287</v>
       </c>
     </row>
-    <row r="129" spans="1:31">
+    <row r="129" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>158</v>
       </c>
@@ -14098,7 +14114,7 @@
         <v>3541</v>
       </c>
     </row>
-    <row r="130" spans="1:31">
+    <row r="130" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>159</v>
       </c>
@@ -14193,7 +14209,7 @@
         <v>2401</v>
       </c>
     </row>
-    <row r="131" spans="1:31">
+    <row r="131" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>160</v>
       </c>
@@ -14288,7 +14304,7 @@
         <v>2389</v>
       </c>
     </row>
-    <row r="132" spans="1:31">
+    <row r="132" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>161</v>
       </c>
@@ -14383,7 +14399,7 @@
         <v>4649</v>
       </c>
     </row>
-    <row r="133" spans="1:31">
+    <row r="133" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>162</v>
       </c>
@@ -14478,7 +14494,7 @@
         <v>2326</v>
       </c>
     </row>
-    <row r="134" spans="1:31">
+    <row r="134" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>163</v>
       </c>
@@ -14573,7 +14589,7 @@
         <v>4396</v>
       </c>
     </row>
-    <row r="135" spans="1:31">
+    <row r="135" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>164</v>
       </c>
@@ -14668,7 +14684,7 @@
         <v>2711</v>
       </c>
     </row>
-    <row r="136" spans="1:31">
+    <row r="136" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>165</v>
       </c>
@@ -14763,7 +14779,7 @@
         <v>1899</v>
       </c>
     </row>
-    <row r="137" spans="1:31">
+    <row r="137" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>166</v>
       </c>
@@ -14858,7 +14874,7 @@
         <v>2611</v>
       </c>
     </row>
-    <row r="138" spans="1:31">
+    <row r="138" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>167</v>
       </c>
@@ -14953,7 +14969,7 @@
         <v>9574</v>
       </c>
     </row>
-    <row r="139" spans="1:31">
+    <row r="139" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>168</v>
       </c>
@@ -15048,7 +15064,7 @@
         <v>10882</v>
       </c>
     </row>
-    <row r="140" spans="1:31">
+    <row r="140" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>169</v>
       </c>
@@ -15143,7 +15159,7 @@
         <v>2057</v>
       </c>
     </row>
-    <row r="141" spans="1:31">
+    <row r="141" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>170</v>
       </c>
@@ -15238,7 +15254,7 @@
         <v>5985</v>
       </c>
     </row>
-    <row r="142" spans="1:31">
+    <row r="142" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>171</v>
       </c>
@@ -15333,7 +15349,7 @@
         <v>3783</v>
       </c>
     </row>
-    <row r="143" spans="1:31">
+    <row r="143" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>172</v>
       </c>
@@ -15428,7 +15444,7 @@
         <v>8897</v>
       </c>
     </row>
-    <row r="144" spans="1:31">
+    <row r="144" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>173</v>
       </c>
@@ -15523,7 +15539,7 @@
         <v>8761</v>
       </c>
     </row>
-    <row r="145" spans="1:31">
+    <row r="145" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>174</v>
       </c>
@@ -15618,7 +15634,7 @@
         <v>4575</v>
       </c>
     </row>
-    <row r="146" spans="1:31">
+    <row r="146" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>175</v>
       </c>
@@ -15677,7 +15693,7 @@
         <v>1386</v>
       </c>
       <c r="T146">
-        <v>8127.000000000001</v>
+        <v>8127.0000000000009</v>
       </c>
       <c r="U146">
         <v>5571</v>
@@ -15713,7 +15729,7 @@
         <v>3264</v>
       </c>
     </row>
-    <row r="147" spans="1:31">
+    <row r="147" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>176</v>
       </c>
@@ -15808,7 +15824,7 @@
         <v>3558</v>
       </c>
     </row>
-    <row r="148" spans="1:31">
+    <row r="148" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>177</v>
       </c>
@@ -15843,7 +15859,7 @@
         <v>1982</v>
       </c>
       <c r="L148">
-        <v>8039.999999999999</v>
+        <v>8039.9999999999991</v>
       </c>
       <c r="M148">
         <v>6533</v>
@@ -15861,7 +15877,7 @@
         <v>1982</v>
       </c>
       <c r="R148">
-        <v>8018.000000000001</v>
+        <v>8018.0000000000009</v>
       </c>
       <c r="S148">
         <v>6541</v>
@@ -15903,7 +15919,7 @@
         <v>6499</v>
       </c>
     </row>
-    <row r="149" spans="1:31">
+    <row r="149" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>178</v>
       </c>
@@ -15998,7 +16014,7 @@
         <v>7460</v>
       </c>
     </row>
-    <row r="150" spans="1:31">
+    <row r="150" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>179</v>
       </c>
@@ -16093,7 +16109,7 @@
         <v>7215</v>
       </c>
     </row>
-    <row r="151" spans="1:31">
+    <row r="151" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>180</v>
       </c>
@@ -16188,7 +16204,7 @@
         <v>5532</v>
       </c>
     </row>
-    <row r="152" spans="1:31">
+    <row r="152" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>181</v>
       </c>
@@ -16283,7 +16299,7 @@
         <v>3215</v>
       </c>
     </row>
-    <row r="153" spans="1:31">
+    <row r="153" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>182</v>
       </c>
@@ -16378,7 +16394,7 @@
         <v>1769</v>
       </c>
     </row>
-    <row r="154" spans="1:31">
+    <row r="154" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>183</v>
       </c>
@@ -16473,7 +16489,7 @@
         <v>2319</v>
       </c>
     </row>
-    <row r="155" spans="1:31">
+    <row r="155" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>184</v>
       </c>
@@ -16568,7 +16584,7 @@
         <v>7095</v>
       </c>
     </row>
-    <row r="156" spans="1:31">
+    <row r="156" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>185</v>
       </c>
@@ -16663,7 +16679,7 @@
         <v>7972</v>
       </c>
     </row>
-    <row r="157" spans="1:31">
+    <row r="157" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>186</v>
       </c>
@@ -16758,7 +16774,7 @@
         <v>6348</v>
       </c>
     </row>
-    <row r="158" spans="1:31">
+    <row r="158" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>187</v>
       </c>
@@ -16853,7 +16869,7 @@
         <v>6694</v>
       </c>
     </row>
-    <row r="159" spans="1:31">
+    <row r="159" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>188</v>
       </c>
@@ -16948,7 +16964,7 @@
         <v>2819</v>
       </c>
     </row>
-    <row r="160" spans="1:31">
+    <row r="160" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>189</v>
       </c>
@@ -17043,7 +17059,7 @@
         <v>2785</v>
       </c>
     </row>
-    <row r="161" spans="1:31">
+    <row r="161" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>190</v>
       </c>
@@ -17138,7 +17154,7 @@
         <v>4163</v>
       </c>
     </row>
-    <row r="162" spans="1:31">
+    <row r="162" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>191</v>
       </c>
@@ -17233,7 +17249,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="163" spans="1:31">
+    <row r="163" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>192</v>
       </c>
@@ -17328,7 +17344,7 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="164" spans="1:31">
+    <row r="164" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>193</v>
       </c>
@@ -17423,7 +17439,7 @@
         <v>2727</v>
       </c>
     </row>
-    <row r="165" spans="1:31">
+    <row r="165" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>194</v>
       </c>
@@ -17518,7 +17534,7 @@
         <v>2051</v>
       </c>
     </row>
-    <row r="166" spans="1:31">
+    <row r="166" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>195</v>
       </c>
@@ -17613,7 +17629,7 @@
         <v>4401</v>
       </c>
     </row>
-    <row r="167" spans="1:31">
+    <row r="167" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>196</v>
       </c>
@@ -17708,7 +17724,7 @@
         <v>4457</v>
       </c>
     </row>
-    <row r="168" spans="1:31">
+    <row r="168" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>197</v>
       </c>
@@ -17803,7 +17819,7 @@
         <v>2803</v>
       </c>
     </row>
-    <row r="169" spans="1:31">
+    <row r="169" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>198</v>
       </c>
@@ -17898,7 +17914,7 @@
         <v>2145</v>
       </c>
     </row>
-    <row r="170" spans="1:31">
+    <row r="170" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>199</v>
       </c>
@@ -17993,7 +18009,7 @@
         <v>4338</v>
       </c>
     </row>
-    <row r="171" spans="1:31">
+    <row r="171" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>200</v>
       </c>
@@ -18088,7 +18104,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="172" spans="1:31">
+    <row r="172" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>201</v>
       </c>
@@ -18183,7 +18199,7 @@
         <v>1718</v>
       </c>
     </row>
-    <row r="173" spans="1:31">
+    <row r="173" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>202</v>
       </c>
@@ -18278,7 +18294,7 @@
         <v>1547</v>
       </c>
     </row>
-    <row r="174" spans="1:31">
+    <row r="174" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>203</v>
       </c>
@@ -18373,7 +18389,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="175" spans="1:31">
+    <row r="175" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>204</v>
       </c>
@@ -18468,7 +18484,7 @@
         <v>2339</v>
       </c>
     </row>
-    <row r="176" spans="1:31">
+    <row r="176" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>205</v>
       </c>
@@ -18563,7 +18579,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="177" spans="1:31">
+    <row r="177" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>206</v>
       </c>
@@ -18658,7 +18674,7 @@
         <v>2878</v>
       </c>
     </row>
-    <row r="178" spans="1:31">
+    <row r="178" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>207</v>
       </c>
@@ -18753,7 +18769,7 @@
         <v>2432</v>
       </c>
     </row>
-    <row r="179" spans="1:31">
+    <row r="179" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>208</v>
       </c>
@@ -18848,7 +18864,7 @@
         <v>2182</v>
       </c>
     </row>
-    <row r="180" spans="1:31">
+    <row r="180" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>209</v>
       </c>
@@ -18943,7 +18959,7 @@
         <v>2895</v>
       </c>
     </row>
-    <row r="181" spans="1:31">
+    <row r="181" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>210</v>
       </c>
@@ -19038,7 +19054,7 @@
         <v>2641</v>
       </c>
     </row>
-    <row r="182" spans="1:31">
+    <row r="182" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>211</v>
       </c>
@@ -19133,7 +19149,7 @@
         <v>3860</v>
       </c>
     </row>
-    <row r="183" spans="1:31">
+    <row r="183" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>212</v>
       </c>
@@ -19228,7 +19244,7 @@
         <v>2242</v>
       </c>
     </row>
-    <row r="184" spans="1:31">
+    <row r="184" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>213</v>
       </c>
@@ -19323,7 +19339,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="185" spans="1:31">
+    <row r="185" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>214</v>
       </c>
@@ -19346,7 +19362,7 @@
         <v>5542</v>
       </c>
       <c r="H185">
-        <v>8087.999999999999</v>
+        <v>8087.9999999999991</v>
       </c>
       <c r="I185">
         <v>5771</v>
@@ -19400,7 +19416,7 @@
         <v>3878</v>
       </c>
       <c r="Z185">
-        <v>8101.000000000001</v>
+        <v>8101.0000000000009</v>
       </c>
       <c r="AA185">
         <v>5771</v>
@@ -19418,7 +19434,7 @@
         <v>3154</v>
       </c>
     </row>
-    <row r="186" spans="1:31">
+    <row r="186" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>215</v>
       </c>
@@ -19513,7 +19529,7 @@
         <v>2231</v>
       </c>
     </row>
-    <row r="187" spans="1:31">
+    <row r="187" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>216</v>
       </c>
@@ -19608,7 +19624,7 @@
         <v>2465</v>
       </c>
     </row>
-    <row r="188" spans="1:31">
+    <row r="188" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>217</v>
       </c>
@@ -19703,7 +19719,7 @@
         <v>4585</v>
       </c>
     </row>
-    <row r="189" spans="1:31">
+    <row r="189" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>218</v>
       </c>
@@ -19762,7 +19778,7 @@
         <v>1409</v>
       </c>
       <c r="T189">
-        <v>8077.999999999999</v>
+        <v>8077.9999999999991</v>
       </c>
       <c r="U189">
         <v>5506</v>
@@ -19798,7 +19814,7 @@
         <v>3302</v>
       </c>
     </row>
-    <row r="190" spans="1:31">
+    <row r="190" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>219</v>
       </c>
@@ -19893,7 +19909,7 @@
         <v>2671</v>
       </c>
     </row>
-    <row r="191" spans="1:31">
+    <row r="191" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>220</v>
       </c>
@@ -19988,7 +20004,7 @@
         <v>2345</v>
       </c>
     </row>
-    <row r="192" spans="1:31">
+    <row r="192" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>221</v>
       </c>
@@ -20083,7 +20099,7 @@
         <v>4928</v>
       </c>
     </row>
-    <row r="193" spans="1:31">
+    <row r="193" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>222</v>
       </c>
@@ -20178,7 +20194,7 @@
         <v>2370</v>
       </c>
     </row>
-    <row r="194" spans="1:31">
+    <row r="194" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>223</v>
       </c>
@@ -20273,7 +20289,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="195" spans="1:31">
+    <row r="195" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>224</v>
       </c>
@@ -20368,7 +20384,7 @@
         <v>38147</v>
       </c>
     </row>
-    <row r="196" spans="1:31">
+    <row r="196" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>225</v>
       </c>
@@ -20463,7 +20479,7 @@
         <v>3798</v>
       </c>
     </row>
-    <row r="197" spans="1:31">
+    <row r="197" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>226</v>
       </c>
@@ -20558,7 +20574,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="198" spans="1:31">
+    <row r="198" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>227</v>
       </c>
@@ -20653,7 +20669,7 @@
         <v>2514</v>
       </c>
     </row>
-    <row r="199" spans="1:31">
+    <row r="199" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>228</v>
       </c>
@@ -20748,7 +20764,7 @@
         <v>22469</v>
       </c>
     </row>
-    <row r="200" spans="1:31">
+    <row r="200" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>229</v>
       </c>
@@ -20843,7 +20859,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="201" spans="1:31">
+    <row r="201" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>230</v>
       </c>
@@ -20878,7 +20894,7 @@
         <v>4838</v>
       </c>
       <c r="L201">
-        <v>8175.000000000001</v>
+        <v>8175.0000000000009</v>
       </c>
       <c r="M201">
         <v>2370</v>
@@ -20938,7 +20954,7 @@
         <v>2449</v>
       </c>
     </row>
-    <row r="202" spans="1:31">
+    <row r="202" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>231</v>
       </c>
@@ -21033,7 +21049,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="203" spans="1:31">
+    <row r="203" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>232</v>
       </c>
@@ -21128,7 +21144,7 @@
         <v>1533</v>
       </c>
     </row>
-    <row r="204" spans="1:31">
+    <row r="204" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>233</v>
       </c>
@@ -21223,7 +21239,7 @@
         <v>3819</v>
       </c>
     </row>
-    <row r="205" spans="1:31">
+    <row r="205" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>234</v>
       </c>
@@ -21318,7 +21334,7 @@
         <v>1694</v>
       </c>
     </row>
-    <row r="206" spans="1:31">
+    <row r="206" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>235</v>
       </c>
@@ -21413,7 +21429,7 @@
         <v>4610</v>
       </c>
     </row>
-    <row r="207" spans="1:31">
+    <row r="207" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>236</v>
       </c>
@@ -21508,7 +21524,7 @@
         <v>1622</v>
       </c>
     </row>
-    <row r="208" spans="1:31">
+    <row r="208" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>237</v>
       </c>
@@ -21603,7 +21619,7 @@
         <v>3015</v>
       </c>
     </row>
-    <row r="209" spans="1:31">
+    <row r="209" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>238</v>
       </c>
@@ -21698,7 +21714,7 @@
         <v>2505</v>
       </c>
     </row>
-    <row r="210" spans="1:31">
+    <row r="210" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>239</v>
       </c>
@@ -21793,7 +21809,7 @@
         <v>4499</v>
       </c>
     </row>
-    <row r="211" spans="1:31">
+    <row r="211" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>240</v>
       </c>
@@ -21888,7 +21904,7 @@
         <v>2771</v>
       </c>
     </row>
-    <row r="212" spans="1:31">
+    <row r="212" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>241</v>
       </c>
@@ -21983,7 +21999,7 @@
         <v>2604</v>
       </c>
     </row>
-    <row r="213" spans="1:31">
+    <row r="213" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>242</v>
       </c>
@@ -22078,7 +22094,7 @@
         <v>1457</v>
       </c>
     </row>
-    <row r="214" spans="1:31">
+    <row r="214" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>243</v>
       </c>
@@ -22098,7 +22114,7 @@
         <v>3112</v>
       </c>
       <c r="G214">
-        <v>8146.000000000001</v>
+        <v>8146.0000000000009</v>
       </c>
       <c r="H214">
         <v>23552</v>
@@ -22173,7 +22189,7 @@
         <v>5441</v>
       </c>
     </row>
-    <row r="215" spans="1:31">
+    <row r="215" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>244</v>
       </c>
@@ -22268,7 +22284,7 @@
         <v>1923</v>
       </c>
     </row>
-    <row r="216" spans="1:31">
+    <row r="216" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>245</v>
       </c>
@@ -22363,7 +22379,7 @@
         <v>2275</v>
       </c>
     </row>
-    <row r="217" spans="1:31">
+    <row r="217" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>246</v>
       </c>
@@ -22458,7 +22474,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="218" spans="1:31">
+    <row r="218" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>247</v>
       </c>
@@ -22553,7 +22569,7 @@
         <v>4530</v>
       </c>
     </row>
-    <row r="219" spans="1:31">
+    <row r="219" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>248</v>
       </c>
@@ -22648,7 +22664,7 @@
         <v>6132</v>
       </c>
     </row>
-    <row r="220" spans="1:31">
+    <row r="220" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>249</v>
       </c>
@@ -22743,7 +22759,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="221" spans="1:31">
+    <row r="221" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>250</v>
       </c>
@@ -22838,7 +22854,7 @@
         <v>1456</v>
       </c>
     </row>
-    <row r="222" spans="1:31">
+    <row r="222" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>251</v>
       </c>
@@ -22933,7 +22949,7 @@
         <v>2244</v>
       </c>
     </row>
-    <row r="223" spans="1:31">
+    <row r="223" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>252</v>
       </c>
@@ -23028,7 +23044,7 @@
         <v>3058</v>
       </c>
     </row>
-    <row r="224" spans="1:31">
+    <row r="224" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>253</v>
       </c>
@@ -23123,7 +23139,7 @@
         <v>2373</v>
       </c>
     </row>
-    <row r="225" spans="1:31">
+    <row r="225" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>254</v>
       </c>
@@ -23218,7 +23234,7 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="226" spans="1:31">
+    <row r="226" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>255</v>
       </c>
@@ -23313,7 +23329,7 @@
         <v>3051</v>
       </c>
     </row>
-    <row r="227" spans="1:31">
+    <row r="227" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>256</v>
       </c>
@@ -23408,7 +23424,7 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="228" spans="1:31">
+    <row r="228" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>257</v>
       </c>
@@ -23503,7 +23519,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="229" spans="1:31">
+    <row r="229" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>258</v>
       </c>
@@ -23598,7 +23614,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="230" spans="1:31">
+    <row r="230" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>259</v>
       </c>
@@ -23693,7 +23709,7 @@
         <v>2483</v>
       </c>
     </row>
-    <row r="231" spans="1:31">
+    <row r="231" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>260</v>
       </c>
@@ -23788,7 +23804,7 @@
         <v>1856</v>
       </c>
     </row>
-    <row r="232" spans="1:31">
+    <row r="232" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>261</v>
       </c>
@@ -23841,7 +23857,7 @@
         <v>4887</v>
       </c>
       <c r="R232">
-        <v>8093.999999999999</v>
+        <v>8093.9999999999991</v>
       </c>
       <c r="S232">
         <v>1045</v>
@@ -23883,7 +23899,7 @@
         <v>2393</v>
       </c>
     </row>
-    <row r="233" spans="1:31">
+    <row r="233" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>262</v>
       </c>
@@ -23978,7 +23994,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="234" spans="1:31">
+    <row r="234" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>263</v>
       </c>
@@ -24073,7 +24089,7 @@
         <v>1711</v>
       </c>
     </row>
-    <row r="235" spans="1:31">
+    <row r="235" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>264</v>
       </c>
@@ -24168,7 +24184,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="236" spans="1:31">
+    <row r="236" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>265</v>
       </c>
@@ -24263,7 +24279,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="237" spans="1:31">
+    <row r="237" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>266</v>
       </c>
@@ -24358,7 +24374,7 @@
         <v>2311</v>
       </c>
     </row>
-    <row r="238" spans="1:31">
+    <row r="238" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>267</v>
       </c>
@@ -24453,7 +24469,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="239" spans="1:31">
+    <row r="239" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>268</v>
       </c>
@@ -24494,7 +24510,7 @@
         <v>2165</v>
       </c>
       <c r="N239">
-        <v>8085.000000000001</v>
+        <v>8085.0000000000009</v>
       </c>
       <c r="O239">
         <v>6101</v>
@@ -24512,7 +24528,7 @@
         <v>2161</v>
       </c>
       <c r="T239">
-        <v>8080.999999999999</v>
+        <v>8080.9999999999991</v>
       </c>
       <c r="U239">
         <v>6101</v>
@@ -24530,7 +24546,7 @@
         <v>2145</v>
       </c>
       <c r="Z239">
-        <v>8085.000000000001</v>
+        <v>8085.0000000000009</v>
       </c>
       <c r="AA239">
         <v>6101</v>
@@ -24548,7 +24564,7 @@
         <v>2158</v>
       </c>
     </row>
-    <row r="240" spans="1:31">
+    <row r="240" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>269</v>
       </c>
@@ -24643,7 +24659,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="241" spans="1:31">
+    <row r="241" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>270</v>
       </c>
@@ -24738,7 +24754,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="242" spans="1:31">
+    <row r="242" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>271</v>
       </c>
@@ -24833,7 +24849,7 @@
         <v>1809</v>
       </c>
     </row>
-    <row r="243" spans="1:31">
+    <row r="243" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>272</v>
       </c>
@@ -24874,7 +24890,7 @@
         <v>2981</v>
       </c>
       <c r="N243">
-        <v>8186.999999999999</v>
+        <v>8186.9999999999991</v>
       </c>
       <c r="O243">
         <v>1878</v>
@@ -24928,7 +24944,7 @@
         <v>3102</v>
       </c>
     </row>
-    <row r="244" spans="1:31">
+    <row r="244" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>273</v>
       </c>
@@ -25023,7 +25039,7 @@
         <v>3090</v>
       </c>
     </row>
-    <row r="245" spans="1:31">
+    <row r="245" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>274</v>
       </c>
@@ -25118,7 +25134,7 @@
         <v>3507</v>
       </c>
     </row>
-    <row r="246" spans="1:31">
+    <row r="246" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>275</v>
       </c>
@@ -25213,7 +25229,7 @@
         <v>2885</v>
       </c>
     </row>
-    <row r="247" spans="1:31">
+    <row r="247" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>276</v>
       </c>
@@ -25308,7 +25324,7 @@
         <v>4147</v>
       </c>
     </row>
-    <row r="248" spans="1:31">
+    <row r="248" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>277</v>
       </c>
@@ -25403,7 +25419,7 @@
         <v>11359</v>
       </c>
     </row>
-    <row r="249" spans="1:31">
+    <row r="249" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>278</v>
       </c>
@@ -25498,7 +25514,7 @@
         <v>7478</v>
       </c>
     </row>
-    <row r="250" spans="1:31">
+    <row r="250" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>279</v>
       </c>
@@ -25593,7 +25609,7 @@
         <v>7734</v>
       </c>
     </row>
-    <row r="251" spans="1:31">
+    <row r="251" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>280</v>
       </c>
@@ -25688,7 +25704,7 @@
         <v>8951</v>
       </c>
     </row>
-    <row r="252" spans="1:31">
+    <row r="252" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>281</v>
       </c>
@@ -25783,7 +25799,7 @@
         <v>3098</v>
       </c>
     </row>
-    <row r="253" spans="1:31">
+    <row r="253" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>282</v>
       </c>
@@ -25878,7 +25894,7 @@
         <v>2497</v>
       </c>
     </row>
-    <row r="254" spans="1:31">
+    <row r="254" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>283</v>
       </c>
@@ -25973,7 +25989,7 @@
         <v>3467</v>
       </c>
     </row>
-    <row r="255" spans="1:31">
+    <row r="255" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>284</v>
       </c>
@@ -26068,7 +26084,7 @@
         <v>9612</v>
       </c>
     </row>
-    <row r="256" spans="1:31">
+    <row r="256" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>285</v>
       </c>
@@ -26163,7 +26179,7 @@
         <v>2483</v>
       </c>
     </row>
-    <row r="257" spans="1:31">
+    <row r="257" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>286</v>
       </c>
@@ -26258,7 +26274,7 @@
         <v>3164</v>
       </c>
     </row>
-    <row r="258" spans="1:31">
+    <row r="258" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>287</v>
       </c>
@@ -26308,7 +26324,7 @@
         <v>1531</v>
       </c>
       <c r="Q258">
-        <v>8026.999999999999</v>
+        <v>8026.9999999999991</v>
       </c>
       <c r="R258">
         <v>11668</v>
@@ -26353,7 +26369,7 @@
         <v>4653</v>
       </c>
     </row>
-    <row r="259" spans="1:31">
+    <row r="259" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>288</v>
       </c>
@@ -26448,7 +26464,7 @@
         <v>2164</v>
       </c>
     </row>
-    <row r="260" spans="1:31">
+    <row r="260" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>289</v>
       </c>
@@ -26543,7 +26559,7 @@
         <v>2609</v>
       </c>
     </row>
-    <row r="261" spans="1:31">
+    <row r="261" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>290</v>
       </c>
@@ -26611,7 +26627,7 @@
         <v>2182</v>
       </c>
       <c r="W261">
-        <v>8080.999999999999</v>
+        <v>8080.9999999999991</v>
       </c>
       <c r="X261">
         <v>5422</v>
@@ -26629,7 +26645,7 @@
         <v>2182</v>
       </c>
       <c r="AC261">
-        <v>8124.000000000001</v>
+        <v>8124.0000000000009</v>
       </c>
       <c r="AD261">
         <v>8711</v>
@@ -26638,7 +26654,7 @@
         <v>7264</v>
       </c>
     </row>
-    <row r="262" spans="1:31">
+    <row r="262" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>291</v>
       </c>
@@ -26733,7 +26749,7 @@
         <v>4377</v>
       </c>
     </row>
-    <row r="263" spans="1:31">
+    <row r="263" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>292</v>
       </c>
@@ -26828,7 +26844,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="264" spans="1:31">
+    <row r="264" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>293</v>
       </c>
@@ -26923,7 +26939,7 @@
         <v>2819</v>
       </c>
     </row>
-    <row r="265" spans="1:31">
+    <row r="265" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>294</v>
       </c>
@@ -27018,7 +27034,7 @@
         <v>1789</v>
       </c>
     </row>
-    <row r="266" spans="1:31">
+    <row r="266" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>295</v>
       </c>
@@ -27113,7 +27129,7 @@
         <v>3201</v>
       </c>
     </row>
-    <row r="267" spans="1:31">
+    <row r="267" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>296</v>
       </c>
@@ -27208,7 +27224,7 @@
         <v>2135</v>
       </c>
     </row>
-    <row r="268" spans="1:31">
+    <row r="268" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>297</v>
       </c>
@@ -27303,7 +27319,7 @@
         <v>7620</v>
       </c>
     </row>
-    <row r="269" spans="1:31">
+    <row r="269" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>298</v>
       </c>
@@ -27398,7 +27414,7 @@
         <v>2110</v>
       </c>
     </row>
-    <row r="270" spans="1:31">
+    <row r="270" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>299</v>
       </c>
@@ -27493,7 +27509,7 @@
         <v>2511</v>
       </c>
     </row>
-    <row r="271" spans="1:31">
+    <row r="271" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>300</v>
       </c>
@@ -27588,7 +27604,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="272" spans="1:31">
+    <row r="272" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>301</v>
       </c>
@@ -27683,7 +27699,7 @@
         <v>3432</v>
       </c>
     </row>
-    <row r="273" spans="1:31">
+    <row r="273" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>302</v>
       </c>
@@ -27778,7 +27794,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="274" spans="1:31">
+    <row r="274" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>303</v>
       </c>
@@ -27831,7 +27847,7 @@
         <v>4023</v>
       </c>
       <c r="R274">
-        <v>8151.999999999999</v>
+        <v>8151.9999999999991</v>
       </c>
       <c r="S274">
         <v>979</v>
@@ -27873,7 +27889,7 @@
         <v>2207</v>
       </c>
     </row>
-    <row r="275" spans="1:31">
+    <row r="275" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>304</v>
       </c>
@@ -27968,7 +27984,7 @@
         <v>2990</v>
       </c>
     </row>
-    <row r="276" spans="1:31">
+    <row r="276" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>305</v>
       </c>
@@ -28063,7 +28079,7 @@
         <v>1838</v>
       </c>
     </row>
-    <row r="277" spans="1:31">
+    <row r="277" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>306</v>
       </c>
@@ -28158,7 +28174,7 @@
         <v>2950</v>
       </c>
     </row>
-    <row r="278" spans="1:31">
+    <row r="278" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>307</v>
       </c>
@@ -28253,7 +28269,7 @@
         <v>3455</v>
       </c>
     </row>
-    <row r="279" spans="1:31">
+    <row r="279" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>308</v>
       </c>
@@ -28348,7 +28364,7 @@
         <v>3527</v>
       </c>
     </row>
-    <row r="280" spans="1:31">
+    <row r="280" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>309</v>
       </c>
@@ -28443,7 +28459,7 @@
         <v>1814</v>
       </c>
     </row>
-    <row r="281" spans="1:31">
+    <row r="281" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>310</v>
       </c>
@@ -28538,12 +28554,12 @@
         <v>1886</v>
       </c>
     </row>
-    <row r="282" spans="1:31">
+    <row r="282" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>311</v>
       </c>
       <c r="B282">
-        <v>8167.999999999999</v>
+        <v>8167.9999999999991</v>
       </c>
       <c r="C282">
         <v>5187</v>
@@ -28591,7 +28607,7 @@
         <v>4652</v>
       </c>
       <c r="R282">
-        <v>8132.999999999999</v>
+        <v>8132.9999999999991</v>
       </c>
       <c r="S282">
         <v>1260</v>
@@ -28633,7 +28649,7 @@
         <v>3142</v>
       </c>
     </row>
-    <row r="283" spans="1:31">
+    <row r="283" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>312</v>
       </c>
@@ -28728,7 +28744,7 @@
         <v>2923</v>
       </c>
     </row>
-    <row r="284" spans="1:31">
+    <row r="284" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>313</v>
       </c>
@@ -28823,7 +28839,7 @@
         <v>3578</v>
       </c>
     </row>
-    <row r="285" spans="1:31">
+    <row r="285" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>314</v>
       </c>
@@ -28918,7 +28934,7 @@
         <v>2786</v>
       </c>
     </row>
-    <row r="286" spans="1:31">
+    <row r="286" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>315</v>
       </c>
@@ -29013,7 +29029,7 @@
         <v>3328</v>
       </c>
     </row>
-    <row r="287" spans="1:31">
+    <row r="287" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>316</v>
       </c>
@@ -29108,7 +29124,7 @@
         <v>2730</v>
       </c>
     </row>
-    <row r="288" spans="1:31">
+    <row r="288" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>317</v>
       </c>
@@ -29203,7 +29219,7 @@
         <v>2498</v>
       </c>
     </row>
-    <row r="289" spans="1:31">
+    <row r="289" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>318</v>
       </c>
@@ -29298,7 +29314,7 @@
         <v>2384</v>
       </c>
     </row>
-    <row r="290" spans="1:31">
+    <row r="290" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>319</v>
       </c>
@@ -29393,7 +29409,7 @@
         <v>2458</v>
       </c>
     </row>
-    <row r="291" spans="1:31">
+    <row r="291" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>320</v>
       </c>
@@ -29488,7 +29504,7 @@
         <v>2523</v>
       </c>
     </row>
-    <row r="292" spans="1:31">
+    <row r="292" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>321</v>
       </c>
@@ -29583,7 +29599,7 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="293" spans="1:31">
+    <row r="293" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>322</v>
       </c>
@@ -29678,7 +29694,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="294" spans="1:31">
+    <row r="294" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>323</v>
       </c>
@@ -29773,7 +29789,7 @@
         <v>2554</v>
       </c>
     </row>
-    <row r="295" spans="1:31">
+    <row r="295" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>324</v>
       </c>
@@ -29868,7 +29884,7 @@
         <v>1743</v>
       </c>
     </row>
-    <row r="296" spans="1:31">
+    <row r="296" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>325</v>
       </c>
@@ -29963,7 +29979,7 @@
         <v>3190</v>
       </c>
     </row>
-    <row r="297" spans="1:31">
+    <row r="297" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>326</v>
       </c>
@@ -29986,7 +30002,7 @@
         <v>5724</v>
       </c>
       <c r="H297">
-        <v>8080.999999999999</v>
+        <v>8080.9999999999991</v>
       </c>
       <c r="I297">
         <v>5775</v>
@@ -30058,7 +30074,7 @@
         <v>3308</v>
       </c>
     </row>
-    <row r="298" spans="1:31">
+    <row r="298" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>327</v>
       </c>
@@ -30153,7 +30169,7 @@
         <v>2352</v>
       </c>
     </row>
-    <row r="299" spans="1:31">
+    <row r="299" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>328</v>
       </c>
@@ -30248,7 +30264,7 @@
         <v>2364</v>
       </c>
     </row>
-    <row r="300" spans="1:31">
+    <row r="300" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>329</v>
       </c>
@@ -30343,7 +30359,7 @@
         <v>2905</v>
       </c>
     </row>
-    <row r="301" spans="1:31">
+    <row r="301" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>330</v>
       </c>
@@ -30438,7 +30454,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="302" spans="1:31">
+    <row r="302" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>331</v>
       </c>
@@ -30533,7 +30549,7 @@
         <v>2457</v>
       </c>
     </row>
-    <row r="303" spans="1:31">
+    <row r="303" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>332</v>
       </c>
@@ -30628,7 +30644,7 @@
         <v>2745</v>
       </c>
     </row>
-    <row r="304" spans="1:31">
+    <row r="304" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>333</v>
       </c>
@@ -30723,7 +30739,7 @@
         <v>3010</v>
       </c>
     </row>
-    <row r="305" spans="1:31">
+    <row r="305" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>334</v>
       </c>
@@ -30818,7 +30834,7 @@
         <v>2243</v>
       </c>
     </row>
-    <row r="306" spans="1:31">
+    <row r="306" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>335</v>
       </c>
@@ -30913,7 +30929,7 @@
         <v>3050</v>
       </c>
     </row>
-    <row r="307" spans="1:31">
+    <row r="307" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>336</v>
       </c>
@@ -31008,7 +31024,7 @@
         <v>2165</v>
       </c>
     </row>
-    <row r="308" spans="1:31">
+    <row r="308" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>337</v>
       </c>
@@ -31103,7 +31119,7 @@
         <v>2088</v>
       </c>
     </row>
-    <row r="309" spans="1:31">
+    <row r="309" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>338</v>
       </c>
@@ -31198,7 +31214,7 @@
         <v>2729</v>
       </c>
     </row>
-    <row r="310" spans="1:31">
+    <row r="310" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>339</v>
       </c>
@@ -31293,7 +31309,7 @@
         <v>1860</v>
       </c>
     </row>
-    <row r="311" spans="1:31">
+    <row r="311" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>340</v>
       </c>
@@ -31388,7 +31404,7 @@
         <v>2218</v>
       </c>
     </row>
-    <row r="312" spans="1:31">
+    <row r="312" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>341</v>
       </c>
@@ -31483,7 +31499,7 @@
         <v>2261</v>
       </c>
     </row>
-    <row r="313" spans="1:31">
+    <row r="313" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>342</v>
       </c>
@@ -31578,7 +31594,7 @@
         <v>2799</v>
       </c>
     </row>
-    <row r="314" spans="1:31">
+    <row r="314" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>343</v>
       </c>
@@ -31673,7 +31689,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="315" spans="1:31">
+    <row r="315" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>344</v>
       </c>
@@ -31768,7 +31784,7 @@
         <v>3138</v>
       </c>
     </row>
-    <row r="316" spans="1:31">
+    <row r="316" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>345</v>
       </c>
@@ -31863,7 +31879,7 @@
         <v>2127</v>
       </c>
     </row>
-    <row r="317" spans="1:31">
+    <row r="317" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>346</v>
       </c>
@@ -31958,7 +31974,7 @@
         <v>1773</v>
       </c>
     </row>
-    <row r="318" spans="1:31">
+    <row r="318" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>347</v>
       </c>
@@ -32053,7 +32069,7 @@
         <v>2476</v>
       </c>
     </row>
-    <row r="319" spans="1:31">
+    <row r="319" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>348</v>
       </c>
@@ -32148,7 +32164,7 @@
         <v>3270</v>
       </c>
     </row>
-    <row r="320" spans="1:31">
+    <row r="320" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>349</v>
       </c>
@@ -32243,7 +32259,7 @@
         <v>2270</v>
       </c>
     </row>
-    <row r="321" spans="1:31">
+    <row r="321" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>350</v>
       </c>
@@ -32338,7 +32354,7 @@
         <v>5990</v>
       </c>
     </row>
-    <row r="322" spans="1:31">
+    <row r="322" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>351</v>
       </c>
@@ -32433,7 +32449,7 @@
         <v>2294</v>
       </c>
     </row>
-    <row r="323" spans="1:31">
+    <row r="323" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>352</v>
       </c>
@@ -32528,7 +32544,7 @@
         <v>1802</v>
       </c>
     </row>
-    <row r="324" spans="1:31">
+    <row r="324" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>353</v>
       </c>
@@ -32623,7 +32639,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="325" spans="1:31">
+    <row r="325" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>354</v>
       </c>
@@ -32718,7 +32734,7 @@
         <v>2551</v>
       </c>
     </row>
-    <row r="326" spans="1:31">
+    <row r="326" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>355</v>
       </c>
@@ -32813,7 +32829,7 @@
         <v>2133</v>
       </c>
     </row>
-    <row r="327" spans="1:31">
+    <row r="327" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>356</v>
       </c>
@@ -32908,7 +32924,7 @@
         <v>2652</v>
       </c>
     </row>
-    <row r="328" spans="1:31">
+    <row r="328" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>357</v>
       </c>
@@ -33009,14 +33025,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18:I33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>358</v>
       </c>
@@ -33045,7 +33063,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>367</v>
       </c>
@@ -33071,7 +33089,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>368</v>
       </c>
@@ -33100,7 +33118,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>369</v>
       </c>
@@ -33129,7 +33147,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>370</v>
       </c>
@@ -33158,7 +33176,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>371</v>
       </c>
@@ -33187,7 +33205,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>372</v>
       </c>
@@ -33216,7 +33234,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>373</v>
       </c>
@@ -33245,7 +33263,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>374</v>
       </c>
@@ -33271,7 +33289,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>375</v>
       </c>
@@ -33300,7 +33318,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>376</v>
       </c>
@@ -33329,7 +33347,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>374</v>
       </c>
@@ -33355,7 +33373,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>377</v>
       </c>
@@ -33384,7 +33402,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>378</v>
       </c>
@@ -33413,7 +33431,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>374</v>
       </c>
@@ -33439,7 +33457,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>379</v>
       </c>
@@ -33468,7 +33486,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>380</v>
       </c>
@@ -33497,7 +33515,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>367</v>
       </c>
@@ -33519,11 +33537,8 @@
       <c r="H18" t="s">
         <v>455</v>
       </c>
-      <c r="I18" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>368</v>
       </c>
@@ -33548,11 +33563,8 @@
       <c r="H19" t="s">
         <v>455</v>
       </c>
-      <c r="I19" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>369</v>
       </c>
@@ -33577,11 +33589,8 @@
       <c r="H20" t="s">
         <v>455</v>
       </c>
-      <c r="I20" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>370</v>
       </c>
@@ -33606,11 +33615,8 @@
       <c r="H21" t="s">
         <v>455</v>
       </c>
-      <c r="I21" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>371</v>
       </c>
@@ -33635,11 +33641,8 @@
       <c r="H22" t="s">
         <v>455</v>
       </c>
-      <c r="I22" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>372</v>
       </c>
@@ -33664,11 +33667,8 @@
       <c r="H23" t="s">
         <v>455</v>
       </c>
-      <c r="I23" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>373</v>
       </c>
@@ -33693,11 +33693,8 @@
       <c r="H24" t="s">
         <v>455</v>
       </c>
-      <c r="I24" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>374</v>
       </c>
@@ -33719,11 +33716,8 @@
       <c r="H25" t="s">
         <v>456</v>
       </c>
-      <c r="I25" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>375</v>
       </c>
@@ -33748,11 +33742,8 @@
       <c r="H26" t="s">
         <v>456</v>
       </c>
-      <c r="I26" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>376</v>
       </c>
@@ -33777,11 +33768,8 @@
       <c r="H27" t="s">
         <v>456</v>
       </c>
-      <c r="I27" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>374</v>
       </c>
@@ -33803,11 +33791,8 @@
       <c r="H28" t="s">
         <v>457</v>
       </c>
-      <c r="I28" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>377</v>
       </c>
@@ -33832,11 +33817,8 @@
       <c r="H29" t="s">
         <v>457</v>
       </c>
-      <c r="I29" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>378</v>
       </c>
@@ -33861,11 +33843,8 @@
       <c r="H30" t="s">
         <v>457</v>
       </c>
-      <c r="I30" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>374</v>
       </c>
@@ -33887,11 +33866,8 @@
       <c r="H31" t="s">
         <v>458</v>
       </c>
-      <c r="I31" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>379</v>
       </c>
@@ -33916,11 +33892,8 @@
       <c r="H32" t="s">
         <v>458</v>
       </c>
-      <c r="I32" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>380</v>
       </c>
@@ -33945,11 +33918,8 @@
       <c r="H33" t="s">
         <v>458</v>
       </c>
-      <c r="I33" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>367</v>
       </c>
@@ -33975,7 +33945,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>368</v>
       </c>
@@ -34004,7 +33974,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>369</v>
       </c>
@@ -34033,7 +34003,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>370</v>
       </c>
@@ -34062,7 +34032,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>371</v>
       </c>
@@ -34091,7 +34061,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>372</v>
       </c>
@@ -34120,7 +34090,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>373</v>
       </c>
@@ -34149,7 +34119,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>374</v>
       </c>
@@ -34175,7 +34145,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>375</v>
       </c>
@@ -34204,7 +34174,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>376</v>
       </c>
@@ -34233,7 +34203,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>374</v>
       </c>
@@ -34259,7 +34229,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>377</v>
       </c>
@@ -34288,7 +34258,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>378</v>
       </c>
@@ -34317,7 +34287,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>374</v>
       </c>
@@ -34343,7 +34313,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>379</v>
       </c>
@@ -34372,7 +34342,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>380</v>
       </c>
@@ -34401,7 +34371,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>367</v>
       </c>
@@ -34427,7 +34397,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>368</v>
       </c>
@@ -34456,7 +34426,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>369</v>
       </c>
@@ -34485,7 +34455,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>370</v>
       </c>
@@ -34514,7 +34484,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>371</v>
       </c>
@@ -34543,7 +34513,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>372</v>
       </c>
@@ -34572,7 +34542,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>373</v>
       </c>
@@ -34601,7 +34571,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>374</v>
       </c>
@@ -34627,7 +34597,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>375</v>
       </c>
@@ -34656,7 +34626,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>376</v>
       </c>
@@ -34685,7 +34655,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>374</v>
       </c>
@@ -34711,7 +34681,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>377</v>
       </c>
@@ -34740,7 +34710,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>378</v>
       </c>
@@ -34769,7 +34739,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>374</v>
       </c>
@@ -34795,7 +34765,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>379</v>
       </c>
@@ -34824,7 +34794,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>380</v>
       </c>
@@ -34853,7 +34823,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>367</v>
       </c>
@@ -34879,7 +34849,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>368</v>
       </c>
@@ -34908,7 +34878,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>369</v>
       </c>
@@ -34937,7 +34907,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>370</v>
       </c>
@@ -34966,7 +34936,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>371</v>
       </c>
@@ -34995,7 +34965,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>372</v>
       </c>
@@ -35024,7 +34994,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>373</v>
       </c>
@@ -35053,7 +35023,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>374</v>
       </c>
@@ -35079,7 +35049,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>375</v>
       </c>
@@ -35108,7 +35078,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>376</v>
       </c>
@@ -35137,7 +35107,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>374</v>
       </c>
@@ -35163,7 +35133,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>377</v>
       </c>
@@ -35192,7 +35162,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>378</v>
       </c>
@@ -35221,7 +35191,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>374</v>
       </c>
@@ -35247,7 +35217,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>379</v>
       </c>
@@ -35276,7 +35246,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>380</v>
       </c>
@@ -35311,14 +35281,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>464</v>
       </c>
@@ -35326,7 +35296,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>465</v>
       </c>
@@ -35334,7 +35304,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>466</v>
       </c>
@@ -35342,12 +35312,12 @@
         <v>474</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>468</v>
       </c>
@@ -35355,7 +35325,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>469</v>
       </c>
@@ -35363,7 +35333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>470</v>
       </c>
@@ -35371,28 +35341,28 @@
         <v>476</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>471</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>366</v>
       </c>
@@ -35403,7 +35373,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>478</v>
       </c>
@@ -35411,7 +35381,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>459</v>
       </c>
@@ -35419,7 +35389,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>461</v>
       </c>
@@ -35427,7 +35397,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>462</v>
       </c>
@@ -35435,7 +35405,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>463</v>
       </c>
@@ -35449,14 +35419,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>479</v>
       </c>
@@ -35470,7 +35440,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>478</v>
       </c>
@@ -35484,7 +35454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>459</v>
       </c>
@@ -35498,7 +35468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>460</v>
       </c>
@@ -35512,7 +35482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>461</v>
       </c>
@@ -35526,7 +35496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>462</v>
       </c>
@@ -35540,7 +35510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>463</v>
       </c>

</xml_diff>